<commit_message>
Working version of 00_Condensed_Improved_v3.R + many versions of performing mediating analysis and variations on cluster analysis in their respective files
</commit_message>
<xml_diff>
--- a/PeerJ-LS2022/Cluster_Big_Five_Statistics.xlsx
+++ b/PeerJ-LS2022/Cluster_Big_Five_Statistics.xlsx
@@ -416,34 +416,34 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>8.6</v>
+        <v>4.3</v>
       </c>
       <c r="C2" t="n">
-        <v>1.39170474787692</v>
+        <v>0.695852373938459</v>
       </c>
       <c r="D2" t="n">
-        <v>5.35</v>
+        <v>2.675</v>
       </c>
       <c r="E2" t="n">
-        <v>1.13670808176853</v>
+        <v>0.568354040884266</v>
       </c>
       <c r="F2" t="n">
-        <v>5.7</v>
+        <v>2.85</v>
       </c>
       <c r="G2" t="n">
-        <v>1.49031964074119</v>
+        <v>0.745159820370595</v>
       </c>
       <c r="H2" t="n">
-        <v>5.85</v>
+        <v>2.925</v>
       </c>
       <c r="I2" t="n">
-        <v>1.63111198750713</v>
+        <v>0.815555993753567</v>
       </c>
       <c r="J2" t="n">
-        <v>6.65</v>
+        <v>3.325</v>
       </c>
       <c r="K2" t="n">
-        <v>1.75544266422131</v>
+        <v>0.877721332110657</v>
       </c>
     </row>
     <row r="3">
@@ -451,34 +451,34 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>4.36842105263158</v>
+        <v>2.18421052631579</v>
       </c>
       <c r="C3" t="n">
-        <v>1.06513047274811</v>
+        <v>0.532565236374054</v>
       </c>
       <c r="D3" t="n">
-        <v>5.57894736842105</v>
+        <v>2.78947368421053</v>
       </c>
       <c r="E3" t="n">
-        <v>1.26120707056922</v>
+        <v>0.630603535284612</v>
       </c>
       <c r="F3" t="n">
-        <v>5.94736842105263</v>
+        <v>2.97368421052632</v>
       </c>
       <c r="G3" t="n">
-        <v>1.43270079882276</v>
+        <v>0.716350399411379</v>
       </c>
       <c r="H3" t="n">
-        <v>6.57894736842105</v>
+        <v>3.28947368421053</v>
       </c>
       <c r="I3" t="n">
-        <v>1.50243467129871</v>
+        <v>0.751217335649356</v>
       </c>
       <c r="J3" t="n">
-        <v>4.78947368421053</v>
+        <v>2.39473684210526</v>
       </c>
       <c r="K3" t="n">
-        <v>1.27274625944674</v>
+        <v>0.636373129723371</v>
       </c>
     </row>
     <row r="4">
@@ -486,34 +486,34 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>6.41666666666667</v>
+        <v>3.20833333333333</v>
       </c>
       <c r="C4" t="n">
-        <v>1.50504203102489</v>
+        <v>0.752521015512443</v>
       </c>
       <c r="D4" t="n">
-        <v>5.83333333333333</v>
+        <v>2.91666666666667</v>
       </c>
       <c r="E4" t="n">
-        <v>1.46680440124618</v>
+        <v>0.733402200623088</v>
       </c>
       <c r="F4" t="n">
-        <v>5.58333333333333</v>
+        <v>2.79166666666667</v>
       </c>
       <c r="G4" t="n">
-        <v>2.35326980770986</v>
+        <v>1.17663490385493</v>
       </c>
       <c r="H4" t="n">
-        <v>8.33333333333333</v>
+        <v>4.16666666666667</v>
       </c>
       <c r="I4" t="n">
-        <v>0.492365963917331</v>
+        <v>0.246182981958666</v>
       </c>
       <c r="J4" t="n">
-        <v>9</v>
+        <v>4.5</v>
       </c>
       <c r="K4" t="n">
-        <v>0.953462589245592</v>
+        <v>0.476731294622796</v>
       </c>
     </row>
     <row r="5">
@@ -521,34 +521,34 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>9.5</v>
+        <v>4.75</v>
       </c>
       <c r="C5" t="n">
-        <v>0.904534033733291</v>
+        <v>0.452267016866645</v>
       </c>
       <c r="D5" t="n">
-        <v>8.16666666666667</v>
+        <v>4.08333333333333</v>
       </c>
       <c r="E5" t="n">
-        <v>1.74945879077104</v>
+        <v>0.874729395385519</v>
       </c>
       <c r="F5" t="n">
-        <v>6.83333333333333</v>
+        <v>3.41666666666667</v>
       </c>
       <c r="G5" t="n">
-        <v>1.46680440124618</v>
+        <v>0.733402200623088</v>
       </c>
       <c r="H5" t="n">
-        <v>7.66666666666667</v>
+        <v>3.83333333333333</v>
       </c>
       <c r="I5" t="n">
-        <v>1.23091490979333</v>
+        <v>0.615457454896664</v>
       </c>
       <c r="J5" t="n">
-        <v>2.66666666666667</v>
+        <v>1.33333333333333</v>
       </c>
       <c r="K5" t="n">
-        <v>0.778498944161523</v>
+        <v>0.389249472080762</v>
       </c>
     </row>
     <row r="6">
@@ -556,34 +556,34 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>7.42857142857143</v>
+        <v>3.71428571428571</v>
       </c>
       <c r="C6" t="n">
-        <v>1.86935964825003</v>
+        <v>0.934679824125017</v>
       </c>
       <c r="D6" t="n">
-        <v>5.92857142857143</v>
+        <v>2.96428571428571</v>
       </c>
       <c r="E6" t="n">
-        <v>1.94003511920178</v>
+        <v>0.97001755960089</v>
       </c>
       <c r="F6" t="n">
-        <v>3.85714285714286</v>
+        <v>1.92857142857143</v>
       </c>
       <c r="G6" t="n">
-        <v>0.770328886519643</v>
+        <v>0.385164443259822</v>
       </c>
       <c r="H6" t="n">
-        <v>4.85714285714286</v>
+        <v>2.42857142857143</v>
       </c>
       <c r="I6" t="n">
-        <v>0.949262293098647</v>
+        <v>0.474631146549323</v>
       </c>
       <c r="J6" t="n">
-        <v>4.21428571428571</v>
+        <v>2.10714285714286</v>
       </c>
       <c r="K6" t="n">
-        <v>1.1217137594956</v>
+        <v>0.560856879747801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>